<commit_message>
Add nrmsd of the updated output from 3d mice
</commit_message>
<xml_diff>
--- a/Project_1/summary.xlsx
+++ b/Project_1/summary.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olufogorehan\Documents\Courses\Graduate\Study_DANCE_Lab\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuhang Lin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F176B474-CCF8-48DC-AC65-5AE1329E089D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Feature</t>
   </si>
@@ -136,20 +137,31 @@
   </si>
   <si>
     <t>impyute (em, loops=10)</t>
+  </si>
+  <si>
+    <t>merge of mice and extratrees_40</t>
+  </si>
+  <si>
+    <t>3D-mice (iter=2, seed=100)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D-mice (iter=1, seed=100)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="176" formatCode="0.0000000_ "/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -160,7 +172,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -219,16 +231,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -547,17 +559,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.625" customWidth="1"/>
-    <col min="2" max="14" width="10.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="10.5" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1428,35 +1441,147 @@
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="O19" s="4" t="e">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.18781890000000001</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.24322659999999999</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.21782019999999999</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.20580490000000001</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.1467821</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.14559250000000001</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.25045699999999999</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0.196493</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0.22881180000000001</v>
+      </c>
+      <c r="K19" s="5">
+        <v>0.2147213</v>
+      </c>
+      <c r="L19" s="5">
+        <v>0.18276020000000001</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0.2105648</v>
+      </c>
+      <c r="N19" s="5">
+        <v>0.26546540000000002</v>
+      </c>
+      <c r="O19" s="4">
         <f>AVERAGE(B19:N19)</f>
-        <v>#DIV/0!</v>
+        <v>0.20740913076923076</v>
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="B20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4" t="e">
-        <f>AVERAGE(B20:N20)</f>
-        <v>#DIV/0!</v>
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="8">
+        <v>0.2028953</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.2625016</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.2355701</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.21756149999999999</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.14724799999999999</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.1457425</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.27084839999999999</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.2311107</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.25933030000000001</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0.24842620000000001</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0.1901919</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0.2330045</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0.2771246</v>
+      </c>
+      <c r="O20" s="4">
+        <f t="shared" ref="O20:O29" si="3">AVERAGE(B20:N20)</f>
+        <v>0.22473504615384615</v>
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="B21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.2024956</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.26413900000000001</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.23642199999999999</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.217616</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.1467599</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.14528869999999999</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.27149210000000001</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.23414409999999999</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.26195269999999998</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0.2517971</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0.19084180000000001</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0.23372229999999999</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0.27795180000000003</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="3"/>
+        <v>0.22574023846153843</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1470,7 +1595,7 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1485,7 +1610,7 @@
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1500,7 +1625,7 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1516,7 +1641,7 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1532,7 +1657,7 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1548,7 +1673,7 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1564,7 +1689,7 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1580,7 +1705,7 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1597,30 +1722,7 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
     </row>
-    <row r="31" spans="1:15">
-      <c r="B31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-    </row>
     <row r="32" spans="1:15">
-      <c r="B32" s="8"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
       <c r="O32" s="4"/>
     </row>
     <row r="33" spans="2:15">
@@ -1651,178 +1753,301 @@
     </row>
     <row r="35" spans="2:15">
       <c r="B35" s="8"/>
-      <c r="F35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
     </row>
     <row r="36" spans="2:15">
       <c r="B36" s="8"/>
-      <c r="F36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
     </row>
     <row r="37" spans="2:15">
-      <c r="F37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
     </row>
     <row r="38" spans="2:15">
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
     </row>
     <row r="39" spans="2:15">
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
     </row>
     <row r="40" spans="2:15">
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
     </row>
     <row r="41" spans="2:15">
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
     </row>
     <row r="42" spans="2:15">
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
     </row>
     <row r="43" spans="2:15">
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
     </row>
     <row r="44" spans="2:15">
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
     </row>
     <row r="45" spans="2:15">
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
     </row>
     <row r="46" spans="2:15">
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
     </row>
     <row r="47" spans="2:15">
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
     </row>
     <row r="48" spans="2:15">
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-    </row>
-    <row r="49" spans="10:15">
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-    </row>
-    <row r="50" spans="10:15">
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-    </row>
-    <row r="51" spans="10:15">
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-    </row>
-    <row r="52" spans="10:15">
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
-    </row>
-    <row r="53" spans="10:15">
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-    </row>
-    <row r="54" spans="10:15">
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-    </row>
-    <row r="55" spans="10:15">
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-    </row>
-    <row r="56" spans="10:15">
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48"/>
+    </row>
+    <row r="49" spans="4:15">
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="O49"/>
+    </row>
+    <row r="50" spans="4:15">
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+    </row>
+    <row r="51" spans="4:15">
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+    </row>
+    <row r="52" spans="4:15">
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="O52"/>
+    </row>
+    <row r="53" spans="4:15">
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+      <c r="O53"/>
+    </row>
+    <row r="54" spans="4:15">
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="O54"/>
+    </row>
+    <row r="55" spans="4:15">
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55"/>
+    </row>
+    <row r="56" spans="4:15">
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
@@ -1830,7 +2055,7 @@
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
     </row>
-    <row r="57" spans="10:15">
+    <row r="57" spans="4:15">
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
@@ -1838,7 +2063,7 @@
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
     </row>
-    <row r="58" spans="10:15">
+    <row r="58" spans="4:15">
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
@@ -1846,7 +2071,7 @@
       <c r="N58" s="4"/>
       <c r="O58" s="4"/>
     </row>
-    <row r="59" spans="10:15">
+    <row r="59" spans="4:15">
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
@@ -1854,7 +2079,7 @@
       <c r="N59" s="4"/>
       <c r="O59" s="4"/>
     </row>
-    <row r="60" spans="10:15">
+    <row r="60" spans="4:15">
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
@@ -1862,7 +2087,7 @@
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
     </row>
-    <row r="61" spans="10:15">
+    <row r="61" spans="4:15">
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
@@ -1870,7 +2095,7 @@
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
     </row>
-    <row r="62" spans="10:15">
+    <row r="62" spans="4:15">
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
@@ -1878,7 +2103,7 @@
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
     </row>
-    <row r="63" spans="10:15">
+    <row r="63" spans="4:15">
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
@@ -1886,7 +2111,7 @@
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
     </row>
-    <row r="64" spans="10:15">
+    <row r="64" spans="4:15">
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>

</xml_diff>